<commit_message>
Lista de Chequeo actualizada
</commit_message>
<xml_diff>
--- a/LISTAS DE CHEQUEO.xlsx
+++ b/LISTAS DE CHEQUEO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SPMP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
   <si>
     <t>PRIORIDAD</t>
   </si>
@@ -302,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,6 +348,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H196"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -676,32 +679,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="13" t="s">
         <v>69</v>
       </c>
@@ -2056,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showWhiteSpace="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2072,32 +2075,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="13" t="s">
         <v>69</v>
       </c>
@@ -2133,6 +2136,12 @@
       <c r="F4" s="14">
         <v>41138</v>
       </c>
+      <c r="G4" s="16">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="B5" s="3">
@@ -2173,8 +2182,8 @@
       <c r="F6" s="14">
         <v>41137</v>
       </c>
-      <c r="G6" s="1">
-        <v>3</v>
+      <c r="G6" s="16">
+        <v>5</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>
@@ -2196,7 +2205,7 @@
       <c r="F7" s="14">
         <v>41137</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="16">
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -2222,7 +2231,7 @@
       <c r="F8" s="14">
         <v>41138</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="45">
       <c r="B9" s="5">
@@ -2240,7 +2249,7 @@
       <c r="F9" s="14">
         <v>41141</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:8" ht="45">
       <c r="B10" s="5">
@@ -2258,7 +2267,7 @@
       <c r="F10" s="14">
         <v>41139</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="45">
       <c r="B11" s="5">
@@ -2276,7 +2285,7 @@
       <c r="F11" s="14">
         <v>41139</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="45">
       <c r="B12" s="5">
@@ -2294,7 +2303,7 @@
       <c r="F12" s="14">
         <v>41139</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="45">
       <c r="B13" s="5">
@@ -2312,7 +2321,7 @@
       <c r="F13" s="14">
         <v>41139</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="45">
       <c r="B14" s="5">
@@ -2330,7 +2339,7 @@
       <c r="F14" s="14">
         <v>41139</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="45">
       <c r="B15" s="5">
@@ -2348,7 +2357,7 @@
       <c r="F15" s="14">
         <v>41139</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="45">
       <c r="B16" s="5">
@@ -2366,9 +2375,9 @@
       <c r="F16" s="14">
         <v>41138</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="5">
         <v>3</v>
       </c>
@@ -2384,8 +2393,14 @@
       <c r="F17" s="14">
         <v>41140</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="30">
+      <c r="G17" s="16">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30">
       <c r="B18" s="5">
         <v>5</v>
       </c>
@@ -2401,6 +2416,7 @@
       <c r="F18" s="14">
         <v>41147</v>
       </c>
+      <c r="G18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2417,7 +2433,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G14">
+  <conditionalFormatting sqref="G4:G18">
     <cfRule type="iconSet" priority="9">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>